<commit_message>
Code made more flexible to abrupt changes
</commit_message>
<xml_diff>
--- a/STABLE CODE/Jupyter/excel.xlsx
+++ b/STABLE CODE/Jupyter/excel.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\0235124\OneDrive - University of Waterloo\Desktop\signodeProjects\pdfParse\pyPDF2\python_code\STABLE CODE\Jupyter\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5290C3A-A9B7-4449-8A1C-CB9861829D0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,22 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>this</t>
+  </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>this1</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -66,6 +86,84 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>200025</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>180975</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>9</xdr:col>
+          <xdr:colOff>200025</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>66675</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1031" name="Button 7" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1031"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="36576" bIns="36576" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-CA" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri"/>
+                  <a:cs typeface="Calibri"/>
+                </a:rPr>
+                <a:t>Button 7</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData fPrintsWithSheet="0"/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -330,13 +428,60 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1031" r:id="rId3" name="Button 7">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[0]!RunPythonScript">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>180975</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>9</xdr:col>
+                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>66675</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
 </worksheet>
 </file>
</xml_diff>